<commit_message>
corrected error in confusioin matrix example
</commit_message>
<xml_diff>
--- a/tabs/confusion_sediments.xlsx
+++ b/tabs/confusion_sediments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kruegeto\Documents\qm4g\tabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087F2D5B-080C-4CEB-9B54-4EF33D749F36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18ACA08-7D38-4AE6-B144-7D05A230BA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{DD3A95E3-CB9D-4DB6-A953-1ECC3D40119A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17430" xr2:uid="{DD3A95E3-CB9D-4DB6-A953-1ECC3D40119A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>20 TRUE negatives</t>
   </si>
   <si>
-    <t>4 FALSE positives (Type II error)</t>
-  </si>
-  <si>
     <t>4 FALSE positives (Type I error)</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>LR- = 2/5</t>
+  </si>
+  <si>
+    <t>4 FALSE negatives (Type II error)</t>
   </si>
 </sst>
 </file>
@@ -458,21 +458,21 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7890625" customWidth="1"/>
-    <col min="2" max="2" width="29.83984375" customWidth="1"/>
-    <col min="3" max="3" width="28.89453125" customWidth="1"/>
-    <col min="4" max="4" width="45.734375" customWidth="1"/>
-    <col min="5" max="5" width="28.5234375" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -481,13 +481,13 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,59 +495,59 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E5" s="1"/>
     </row>

</xml_diff>